<commit_message>
Excel parse stage #2
</commit_message>
<xml_diff>
--- a/functions/views/test.xlsx
+++ b/functions/views/test.xlsx
@@ -20,33 +20,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t xml:space="preserve">USN</t>
+  </si>
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">USN</t>
-  </si>
-  <si>
     <t xml:space="preserve">Room</t>
   </si>
   <si>
     <t xml:space="preserve">Seat No</t>
   </si>
   <si>
+    <t xml:space="preserve">1si16cs01</t>
+  </si>
+  <si>
     <t xml:space="preserve">KPS</t>
   </si>
   <si>
+    <t xml:space="preserve">1si16cs02</t>
+  </si>
+  <si>
     <t xml:space="preserve">ADI</t>
   </si>
   <si>
+    <t xml:space="preserve">1si16cs03</t>
+  </si>
+  <si>
     <t xml:space="preserve">NAT</t>
   </si>
   <si>
+    <t xml:space="preserve">1si16cs04</t>
+  </si>
+  <si>
     <t xml:space="preserve">GS</t>
   </si>
   <si>
+    <t xml:space="preserve">1si16cs05</t>
+  </si>
+  <si>
     <t xml:space="preserve">NIK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1si16cs06</t>
   </si>
   <si>
     <t xml:space="preserve">SHK</t>
@@ -64,6 +82,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -123,8 +142,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -148,7 +171,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -171,11 +194,11 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>46</v>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -185,11 +208,11 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2</v>
@@ -199,11 +222,11 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>66</v>
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3</v>
@@ -213,11 +236,11 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>43</v>
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>4</v>
@@ -227,11 +250,11 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>69</v>
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>5</v>
@@ -241,11 +264,11 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>10</v>
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>6</v>

</xml_diff>